<commit_message>
Actualizando todas las campañas a la fecha
</commit_message>
<xml_diff>
--- a/camino_cumbre/camino_cumbre.xlsx
+++ b/camino_cumbre/camino_cumbre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/camino_cumbre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43183CD1-A165-4F49-A9F2-7D6D10CDCCEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61112005-90D2-BC48-8446-D4F70C30DDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -122,13 +122,13 @@
     <t>Mes_3_Prod</t>
   </si>
   <si>
+    <t>EVELYN CAROLINA VENEGAS IÐIGUEZ</t>
+  </si>
+  <si>
     <t>ANA LAURA CONTRERAS IÐIGUEZ</t>
   </si>
   <si>
-    <t>EVELYN CAROLINA VENEGAS IÐIGUEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LAURA DOLORES MONTAÐO </t>
+    <t>LAURA DOLORES MONTAÐO MONTAÐO</t>
   </si>
 </sst>
 </file>
@@ -265,7 +265,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -291,33 +291,75 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0315DA01-7635-3B4E-915F-54A381A18AE8}"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <border>
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color indexed="64"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color indexed="64"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color indexed="64"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
@@ -442,6 +484,38 @@
         </top>
         <bottom style="hair">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="hair">
+          <color indexed="64"/>
+        </left>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top style="hair">
+          <color indexed="64"/>
+        </top>
+        <bottom style="hair">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -514,47 +588,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -611,7 +644,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -624,12 +657,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -905,29 +932,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K21" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="A1:K21" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="LAURA DOLORES MONTAÑO MONTAÑO"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K21" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="A1:K21" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K39">
     <sortCondition descending="1" ref="G1:G39"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="16" dataCellStyle="Normal 2"/>
-    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="13" dataCellStyle="Millares"/>
-    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="12" dataCellStyle="Normal 2"/>
-    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="11" dataCellStyle="Normal 2"/>
-    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="10" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="9" dataCellStyle="Millares">
+    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="19"/>
+    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="18" dataCellStyle="Normal 2"/>
+    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="0" dataCellStyle="Normal 2"/>
+    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="15" dataCellStyle="Normal 2"/>
+    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="12" dataCellStyle="Millares">
       <calculatedColumnFormula>IF(G2&gt;=(E2*4),"EN META","POR DEBAJO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1255,7 +1276,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C1" sqref="C1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1305,7 +1326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" hidden="1">
+    <row r="2" spans="1:11" ht="18">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1313,27 +1334,27 @@
         <v>110453</v>
       </c>
       <c r="C2" s="6">
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D2" s="10">
         <v>45600</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="14">
         <v>14</v>
       </c>
       <c r="F2" s="7">
         <v>5</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="15">
         <v>43</v>
       </c>
-      <c r="H2" s="13">
+      <c r="H2" s="12">
         <v>5.5</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="12">
         <v>1</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="12">
         <v>5.5</v>
       </c>
       <c r="K2" s="11" t="str">
@@ -1341,7 +1362,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1350,27 +1371,27 @@
       </c>
       <c r="C3" s="6">
         <f>C2</f>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D3" s="10">
         <v>45497</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="14">
         <v>18</v>
       </c>
       <c r="F3" s="7">
         <v>6</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="15">
         <v>27.5</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>7</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="12">
         <v>4</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <v>3</v>
       </c>
       <c r="K3" s="8" t="str">
@@ -1378,7 +1399,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1">
+    <row r="4" spans="1:11">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1387,27 +1408,27 @@
       </c>
       <c r="C4" s="6">
         <f t="shared" ref="C4:C21" si="1">C3</f>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D4" s="10">
         <v>45639</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="14">
         <v>13</v>
       </c>
       <c r="F4" s="7">
         <v>5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="15">
         <v>22</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="12">
         <v>8</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="12">
         <v>0.5</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="12">
         <v>3.5</v>
       </c>
       <c r="K4" s="8" t="str">
@@ -1415,7 +1436,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1424,27 +1445,27 @@
       </c>
       <c r="C5" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D5" s="10">
         <v>45583</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="14">
         <v>15</v>
       </c>
       <c r="F5" s="7">
         <v>5</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="15">
         <v>21.5</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="12">
         <v>7</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="12">
         <v>0.5</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="12">
         <v>0</v>
       </c>
       <c r="K5" s="8" t="str">
@@ -1452,36 +1473,36 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1">
-      <c r="A6" s="14" t="s">
-        <v>29</v>
+    <row r="6" spans="1:11">
+      <c r="A6" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="5">
         <v>109998</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D6" s="10">
         <v>45596</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="14">
         <v>15</v>
       </c>
       <c r="F6" s="7">
         <v>5</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="15">
         <v>19.5</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="12">
         <v>5</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <v>2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <v>2</v>
       </c>
       <c r="K6" s="8" t="str">
@@ -1489,7 +1510,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1498,27 +1519,27 @@
       </c>
       <c r="C7" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D7" s="10">
         <v>45560</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="14">
         <v>16</v>
       </c>
       <c r="F7" s="7">
         <v>6</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="15">
         <v>19</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="12">
         <v>6</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="12">
         <v>2.5</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="12">
         <v>3</v>
       </c>
       <c r="K7" s="8" t="str">
@@ -1526,7 +1547,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1535,27 +1556,27 @@
       </c>
       <c r="C8" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D8" s="10">
         <v>45562</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="14">
         <v>16</v>
       </c>
       <c r="F8" s="7">
         <v>6</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="15">
         <v>18.5</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="12">
         <v>7.5</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="12">
         <v>2</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="12">
         <v>0</v>
       </c>
       <c r="K8" s="8" t="str">
@@ -1563,7 +1584,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1">
+    <row r="9" spans="1:11">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
@@ -1572,27 +1593,27 @@
       </c>
       <c r="C9" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D9" s="10">
         <v>45863</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="14">
         <v>6</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="15">
         <v>13.5</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="12">
         <v>5.5</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="12">
         <v>1</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
         <v>2</v>
       </c>
       <c r="K9" s="8" t="str">
@@ -1600,7 +1621,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1">
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1609,27 +1630,27 @@
       </c>
       <c r="C10" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D10" s="10">
         <v>45525</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="14">
         <v>17</v>
       </c>
       <c r="F10" s="7">
         <v>6</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="15">
         <v>12.5</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="12">
         <v>4.5</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="12">
         <v>2</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
         <v>0</v>
       </c>
       <c r="K10" s="8" t="str">
@@ -1637,7 +1658,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1">
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1646,27 +1667,27 @@
       </c>
       <c r="C11" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D11" s="10">
         <v>45944</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="14">
         <v>3</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="15">
         <v>12</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="12">
         <v>8.5</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="12">
         <v>2</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
         <v>1.5</v>
       </c>
       <c r="K11" s="8" t="str">
@@ -1674,7 +1695,7 @@
         <v>EN META</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1683,27 +1704,27 @@
       </c>
       <c r="C12" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D12" s="10">
         <v>45707</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="14">
         <v>11</v>
       </c>
       <c r="F12" s="7">
         <v>4</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="15">
         <v>11.5</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="12">
         <v>6</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="12">
         <v>3</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
         <v>0</v>
       </c>
       <c r="K12" s="8" t="str">
@@ -1711,36 +1732,36 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1">
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="5">
         <v>113450</v>
       </c>
       <c r="C13" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D13" s="10">
         <v>45852</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="14">
         <v>6</v>
       </c>
       <c r="F13" s="7">
         <v>2</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="15">
         <v>10.5</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="12">
         <v>7</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="12">
         <v>2</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="12">
         <v>1</v>
       </c>
       <c r="K13" s="8" t="str">
@@ -1748,7 +1769,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1">
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1757,27 +1778,27 @@
       </c>
       <c r="C14" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D14" s="10">
         <v>45806</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="14">
         <v>8</v>
       </c>
       <c r="F14" s="7">
         <v>3</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="15">
         <v>10.5</v>
       </c>
-      <c r="H14" s="13">
+      <c r="H14" s="12">
         <v>5.5</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="12">
         <v>2</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
         <v>1.5</v>
       </c>
       <c r="K14" s="8" t="str">
@@ -1785,7 +1806,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1">
+    <row r="15" spans="1:11">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1794,27 +1815,27 @@
       </c>
       <c r="C15" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D15" s="10">
         <v>45986</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="14">
         <v>2</v>
       </c>
       <c r="F15" s="7">
         <v>1</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="15">
         <v>9</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="12">
         <v>8</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="12">
         <v>1</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="12">
         <v>0</v>
       </c>
       <c r="K15" s="8" t="str">
@@ -1822,7 +1843,7 @@
         <v>EN META</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1">
+    <row r="16" spans="1:11">
       <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1831,27 +1852,27 @@
       </c>
       <c r="C16" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D16" s="10">
         <v>45736</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="14">
         <v>10</v>
       </c>
       <c r="F16" s="7">
         <v>4</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="15">
         <v>9</v>
       </c>
-      <c r="H16" s="13">
+      <c r="H16" s="12">
         <v>5.5</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="12">
         <v>0</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="12">
         <v>1.5</v>
       </c>
       <c r="K16" s="8" t="str">
@@ -1859,7 +1880,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1">
+    <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
@@ -1868,27 +1889,27 @@
       </c>
       <c r="C17" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D17" s="10">
         <v>45904</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="14">
         <v>4</v>
       </c>
       <c r="F17" s="7">
         <v>2</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="15">
         <v>8</v>
       </c>
-      <c r="H17" s="13">
+      <c r="H17" s="12">
         <v>6</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="12">
         <v>0</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="12">
         <v>1</v>
       </c>
       <c r="K17" s="8" t="str">
@@ -1896,7 +1917,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1">
+    <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
@@ -1905,27 +1926,27 @@
       </c>
       <c r="C18" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D18" s="10">
         <v>45930</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="14">
         <v>4</v>
       </c>
       <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="15">
         <v>6.5</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H18" s="12">
         <v>4.5</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="12">
         <v>2</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="12">
         <v>0</v>
       </c>
       <c r="K18" s="8" t="str">
@@ -1933,7 +1954,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1">
+    <row r="19" spans="1:11">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -1942,27 +1963,27 @@
       </c>
       <c r="C19" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D19" s="10">
         <v>46010</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="14">
         <v>1</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="15">
         <v>6</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="12">
         <v>6</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="12">
         <v>0</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="12">
         <v>0</v>
       </c>
       <c r="K19" s="8" t="str">
@@ -1979,27 +2000,27 @@
       </c>
       <c r="C20" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D20" s="10">
         <v>45776</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="14">
         <v>9</v>
       </c>
       <c r="F20" s="7">
         <v>3</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="15">
         <v>6</v>
       </c>
-      <c r="H20" s="13">
+      <c r="H20" s="12">
         <v>4</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="12">
         <v>0</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="12">
         <v>2</v>
       </c>
       <c r="K20" s="8" t="str">
@@ -2007,7 +2028,7 @@
         <v>POR DEBAJO</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1">
+    <row r="21" spans="1:11">
       <c r="A21" s="9" t="s">
         <v>12</v>
       </c>
@@ -2016,27 +2037,27 @@
       </c>
       <c r="C21" s="6">
         <f t="shared" si="1"/>
-        <v>46017</v>
+        <v>46022</v>
       </c>
       <c r="D21" s="10">
         <v>45950</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="14">
         <v>3</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="15">
         <v>4</v>
       </c>
-      <c r="H21" s="13">
+      <c r="H21" s="12">
         <v>4</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="12">
         <v>0</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="12">
         <v>0</v>
       </c>
       <c r="K21" s="8" t="str">
@@ -2045,33 +2066,38 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C21 E2:F21">
-    <cfRule type="expression" dxfId="8" priority="15" stopIfTrue="1">
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+      <formula>#REF!&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C21 F2:F21">
+    <cfRule type="expression" dxfId="10" priority="23" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D21">
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
-    <cfRule type="expression" dxfId="6" priority="10" stopIfTrue="1">
+  <conditionalFormatting sqref="E2:E21">
+    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H21">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$Z2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J21">
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I21">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$AA2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2081,16 +2107,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K21">
-    <cfRule type="expression" dxfId="2" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="21" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="22" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>#REF!&lt;&gt;""</formula>
+  <conditionalFormatting sqref="G2:G21">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Corrigiendo rutas de imagenes de TODAS las campañas
</commit_message>
<xml_diff>
--- a/camino_cumbre/camino_cumbre.xlsx
+++ b/camino_cumbre/camino_cumbre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diego/Desktop/ ANTIGRAVITY/camino_cumbre/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61112005-90D2-BC48-8446-D4F70C30DDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FD1D3B-F756-8F46-B113-1A57B23398CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16140" xr2:uid="{1DAE931C-7393-E748-9117-F29D24551926}"/>
   </bookViews>
@@ -305,64 +305,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{0315DA01-7635-3B4E-915F-54A381A18AE8}"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="#,##0.0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="hair">
-          <color indexed="64"/>
-        </left>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top style="hair">
-          <color indexed="64"/>
-        </top>
-        <bottom style="hair">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <border>
         <left style="thin">
@@ -588,6 +531,47 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -932,23 +916,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K21" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}" name="Tabla1354" displayName="Tabla1354" ref="A1:K21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
   <autoFilter ref="A1:K21" xr:uid="{3F406AE1-44E1-3545-A7F7-9AB7AD7F1C0E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K39">
     <sortCondition descending="1" ref="G1:G39"/>
   </sortState>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="19"/>
-    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="18" dataCellStyle="Normal 2"/>
-    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="17" dataCellStyle="Normal 2"/>
-    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="0" dataCellStyle="Normal 2"/>
-    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="15" dataCellStyle="Normal 2"/>
-    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="14" dataCellStyle="Normal 2"/>
-    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="12" dataCellStyle="Millares">
+    <tableColumn id="1" xr3:uid="{F64D903D-9F21-1C46-8ECA-63392820498E}" name="Asesor" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{E38F8F07-E36B-CC43-B077-DF828B75CE31}" name="Clave" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{12677A66-E491-A149-827F-A27FD283E2FE}" name="Fecha_Corte" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{7B920709-BCF4-6E42-BB63-55BF01110007}" name="Fecha_Conexion" dataDxfId="17" dataCellStyle="Normal 2"/>
+    <tableColumn id="9" xr3:uid="{EB5FBA11-D0FE-794C-8F1D-3C3492AB053A}" name="Mes_Asesor" dataDxfId="16" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{17B4B670-463A-8F40-996C-94559C2C6156}" name="Trimestre" dataDxfId="15"/>
+    <tableColumn id="6" xr3:uid="{A4DA8ED3-2571-AD46-AEE7-65DE2102D661}" name="Polizas_Totales" dataDxfId="14" dataCellStyle="Normal 2"/>
+    <tableColumn id="16" xr3:uid="{2103F9BE-FF32-BF42-B491-685E796B7946}" name="Mes_1_Prod" dataDxfId="13" dataCellStyle="Normal 2"/>
+    <tableColumn id="18" xr3:uid="{E43E2E5F-4B97-DC43-90D1-8A6AB3D848E9}" name="Mes_2_Prod" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="17" xr3:uid="{3B87E0D8-ACE3-034E-9A51-908E049FE5F8}" name="Mes_3_Prod" dataDxfId="11" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{9128F4F2-9D5B-114E-AFF8-D23C1B15D538}" name="Estatus_meta" dataDxfId="10" dataCellStyle="Millares">
       <calculatedColumnFormula>IF(G2&gt;=(E2*4),"EN META","POR DEBAJO")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2067,37 +2051,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="11" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C21 F2:F21">
-    <cfRule type="expression" dxfId="10" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="23" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D21">
-    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E21">
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>$B2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G21">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H21">
-    <cfRule type="expression" dxfId="6" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$Z2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:J21">
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
       <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I21">
-    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND($B2&lt;&gt;"",$AA2&lt;1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2107,16 +2096,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K21">
-    <cfRule type="expression" dxfId="3" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="21" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="22" stopIfTrue="1">
       <formula>#REF!&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G21">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>$B2&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>